<commit_message>
updated connections and connector locations
</commit_message>
<xml_diff>
--- a/Documents/Connections.xlsx
+++ b/Documents/Connections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54ddf2402abfc0be/Clients/002 - Prof Shen/05 Preliminary/15 Prosthesis PCBA/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54ddf2402abfc0be/Clients/002 - Prof Shen/05 Preliminary/15 Prosthesis PCBA/ECAD/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C60A68B8-B16A-4175-9938-55F3A5A70494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C60A68B8-B16A-4175-9938-55F3A5A70494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7432373-9D57-431C-9E7A-C262034C935F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{961FE144-C187-4163-B7E9-D83607D1C7D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Note: The below does not correlate to any physical pin numbers. This is just a reference for figuring out how many pins are needed for the connectors. Brett can assign pins as he sees best.</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Mag Encoder</t>
+  </si>
+  <si>
+    <t>STO</t>
   </si>
 </sst>
 </file>
@@ -377,18 +380,6 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -416,6 +407,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,9 +1207,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1244,7 +1247,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1350,7 +1353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1492,7 +1495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1503,7 +1506,7 @@
   <dimension ref="B2:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1527,355 +1530,357 @@
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="4"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13"/>
-      <c r="R7" s="10" t="s">
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="R7" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13"/>
-      <c r="R8" s="14" t="s">
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="R8" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13"/>
-      <c r="R9" s="16" t="s">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="R9" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="N11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="16" t="s">
+      <c r="O11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="N12" s="16" t="s">
+      <c r="N12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="16" t="s">
+      <c r="O12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
+      <c r="F13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.4">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="V16" s="22" t="s">
+      <c r="V16" s="18" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>